<commit_message>
Update timetable export logic and fix import issues
</commit_message>
<xml_diff>
--- a/public/book1.xlsx
+++ b/public/book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edaml\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edaml\OneDrive\Desktop\New folder\TKB\timetable-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D8D4D7-A22D-4818-BE20-5289B6A985B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F098C-86B4-4038-90AD-8715A4ADA2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -828,54 +828,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -884,100 +836,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,25 +863,156 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -1297,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C225E10A-CF30-4364-9CE7-1DEA20E0E493}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K5" sqref="J4:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1308,20 +1307,20 @@
     <col min="3" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1347,524 +1346,523 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="50"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="27" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="40"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="30" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="53"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="20" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="54"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="52"/>
-    </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="39"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="27" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="40"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="30" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="20" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="54"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
       <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="52"/>
-    </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="34"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="38"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="39"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="27" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="40"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="53"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="54"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="52"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="38"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="39"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="27" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="40"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="30" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="53"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="54"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="52"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="38"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="27" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="40"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="30" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="53"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="20" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="54"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
     </row>
     <row r="33" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="52"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="38"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="39"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="27" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="40"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25"/>
     </row>
     <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="30" t="s">
+      <c r="A37" s="13"/>
+      <c r="B37" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="53"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="13"/>
+      <c r="B38" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="54"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
     </row>
     <row r="39" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="42"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="52"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="38"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="39"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="22"/>
     </row>
     <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="27" t="s">
+      <c r="A42" s="13"/>
+      <c r="B42" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="40"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="25"/>
     </row>
     <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="46"/>
-      <c r="B43" s="30" t="s">
+      <c r="A43" s="13"/>
+      <c r="B43" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="53"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
-      <c r="B44" s="20" t="s">
+      <c r="A44" s="13"/>
+      <c r="B44" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="54"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="31"/>
     </row>
     <row r="45" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="52"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Ẩn nút xuất PDF và cập nhật định dạng Excel
</commit_message>
<xml_diff>
--- a/public/book1.xlsx
+++ b/public/book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edaml\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edaml\OneDrive\Desktop\New folder\TKB\timetable-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA66FC-5CFF-431A-B890-DA6FF4E2A8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314E7846-FC1B-4FAD-B52D-B2803E65EE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -530,20 +530,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,6 +645,14 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -668,18 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C225E10A-CF30-4364-9CE7-1DEA20E0E493}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -973,7 +960,7 @@
     <col min="3" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="25.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>8</v>
       </c>
@@ -982,640 +969,636 @@
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="34">
+      <c r="G1" s="29">
         <f ca="1">TODAY()</f>
-        <v>45926</v>
-      </c>
-      <c r="H1" s="35"/>
-    </row>
-    <row r="2" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+        <v>45939</v>
+      </c>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+    </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
-    </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="6" t="s">
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="18"/>
-    </row>
-    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="9" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
-    </row>
-    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-    </row>
-    <row r="33" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C37" s="22"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
-    </row>
-    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="27"/>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="21"/>
-    </row>
-    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="24"/>
-    </row>
-    <row r="39" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="27"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="12"/>
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="15"/>
+      <c r="B41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
+      <c r="B42" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="21"/>
-    </row>
-    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="B43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="24"/>
-    </row>
-    <row r="45" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="27"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A27:A32"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: Add Valorant league filtering - Only show major tournaments (Champions, Pacific, Masters, APAC, SEA, OVS, ON Live)
</commit_message>
<xml_diff>
--- a/public/book1.xlsx
+++ b/public/book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edaml\OneDrive\Desktop\New folder\TKB\timetable-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314E7846-FC1B-4FAD-B52D-B2803E65EE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC33BAF3-6589-4C38-92B9-05F8915B3D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="898" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -949,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C225E10A-CF30-4364-9CE7-1DEA20E0E493}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -960,645 +960,646 @@
     <col min="3" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" ht="25.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29">
         <f ca="1">TODAY()</f>
-        <v>45939</v>
-      </c>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+        <v>45956</v>
+      </c>
+      <c r="H2" s="30"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
+      <c r="B12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
+      <c r="B18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="C20" s="22"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="35" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="18"/>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
+      <c r="B30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="24"/>
-    </row>
-    <row r="32" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33" t="s">
+      <c r="C32" s="22"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="27"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="15"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="18"/>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15"/>
     </row>
     <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
+      <c r="B36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
-    </row>
-    <row r="38" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
+      <c r="C38" s="22"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="24"/>
+    </row>
+    <row r="39" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="27"/>
-    </row>
-    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="27"/>
+    </row>
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="15"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="21"/>
+      <c r="B42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="24"/>
-    </row>
-    <row r="44" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
+      <c r="C44" s="22"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="24"/>
+    </row>
+    <row r="45" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="27"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A33"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>